<commit_message>
added styling with events on the exported excel sheet
</commit_message>
<xml_diff>
--- a/school-programs.xlsx
+++ b/school-programs.xlsx
@@ -61,13 +61,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -89,8 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -392,10 +404,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,24 +419,42 @@
     <col min="5" max="5" width="26.993408" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>86</v>
       </c>
@@ -441,7 +471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>87</v>
       </c>
@@ -458,7 +488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>92</v>
       </c>

</xml_diff>